<commit_message>
bug fix suggested by WAH Spekkink
</commit_message>
<xml_diff>
--- a/ExcelCsvImporter/private/ExcelTest.xlsx
+++ b/ExcelCsvImporter/private/ExcelTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Author</t>
   </si>
@@ -58,9 +58,6 @@
     <t> 400 copies</t>
   </si>
   <si>
-    <t>Authors</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Glaston, John; Smith, Humphrey</t>
   </si>
   <si>
-    <t>Lemarck, Christian; Bloor,Mary; Van Dijke, Leo</t>
-  </si>
-  <si>
     <t>Complex systems in urban settings</t>
   </si>
   <si>
@@ -107,6 +101,21 @@
   </si>
   <si>
     <t>Oceanography</t>
+  </si>
+  <si>
+    <t>Followers</t>
+  </si>
+  <si>
+    <t>Person being followed</t>
+  </si>
+  <si>
+    <t>Barack, Obama</t>
+  </si>
+  <si>
+    <t>Glaston, John</t>
+  </si>
+  <si>
+    <t>Lemarck, Christian; Bloor, Mary; Van Dijke, Leo</t>
   </si>
 </sst>
 </file>
@@ -498,7 +507,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,10 +636,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,63 +647,75 @@
     <col min="1" max="2" width="35.5703125" style="5"/>
     <col min="3" max="3" width="5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="5">
         <v>1972</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5">
         <v>1968</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5">
         <v>1980</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -706,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -717,10 +738,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1">
         <v>22</v>
@@ -728,10 +749,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -739,10 +760,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -750,10 +771,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>21</v>
@@ -761,10 +782,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -772,10 +793,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -783,10 +804,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>25</v>
@@ -794,10 +815,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>55</v>
@@ -805,10 +826,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>12</v>

</xml_diff>

<commit_message>
added temporal networks to the Excel / csv converter
</commit_message>
<xml_diff>
--- a/ExcelCsvImporter/private/ExcelTest.xlsx
+++ b/ExcelCsvImporter/private/ExcelTest.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Author</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Lemarck, Christian; Bloor, Mary; Van Dijke, Leo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>1972-01-01,1972-01-15</t>
+  </si>
+  <si>
+    <t>1972-01-13,1972-01-19</t>
+  </si>
+  <si>
+    <t>1972-01-07,1972-01-28</t>
   </si>
 </sst>
 </file>
@@ -185,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -201,6 +213,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -639,13 +654,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="35.5703125" style="5"/>
-    <col min="3" max="3" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
@@ -657,8 +672,8 @@
       <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
+      <c r="C1" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>14</v>
@@ -667,15 +682,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5">
-        <v>1972</v>
+      <c r="C2" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>15</v>
@@ -684,15 +699,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5">
-        <v>1968</v>
+      <c r="C3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>16</v>
@@ -701,15 +716,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5">
-        <v>1980</v>
+      <c r="C4" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>22</v>
@@ -720,6 +735,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>